<commit_message>
Atualizando resultado dos testes no Excel
</commit_message>
<xml_diff>
--- a/tests/Resultado_testes_prototipo1.xlsx
+++ b/tests/Resultado_testes_prototipo1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferdd Nando\Downloads\Projeto - MicroGram\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97d9477719a18e01/Documentos/PythonProjects/Projeto - MicroGram/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CCCC5F-8193-4B9C-A2F2-DE07F19519A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{14CCCC5F-8193-4B9C-A2F2-DE07F19519A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9C4E15-5004-4957-AD45-B2CCFA129D0F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D19105F-3011-4D07-8639-B34B4B833646}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3D19105F-3011-4D07-8639-B34B4B833646}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -320,9 +320,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -649,472 +648,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65891157-909B-4FC9-B822-30361C061FC8}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="100.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="C32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>